<commit_message>
add of cs file
</commit_message>
<xml_diff>
--- a/Documents/Document.xlsx
+++ b/Documents/Document.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
-    <sheet name="ネイティブサイド仕様" sheetId="2" r:id="rId2"/>
-    <sheet name="サーバサイド仕様" sheetId="3" r:id="rId3"/>
+    <sheet name="環境構築" sheetId="6" r:id="rId2"/>
+    <sheet name="ネイティブサイド仕様" sheetId="2" r:id="rId3"/>
+    <sheet name="サーバサイド仕様" sheetId="3" r:id="rId4"/>
+    <sheet name="DB設計" sheetId="4" r:id="rId5"/>
+    <sheet name="API" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="117">
   <si>
     <t>概要兼メモ</t>
     <rPh sb="0" eb="2">
@@ -101,13 +104,600 @@
       <t>シヨウスル</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ネイティブサイドメモ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ギルド、ルーム、個人ルームチャットの３種類</t>
+    <rPh sb="8" eb="10">
+      <t>コジン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チャット後10秒毎に表示し、時間が進むと1時間毎の表示、日の表示に変更</t>
+    <rPh sb="7" eb="8">
+      <t>ビョウ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ゴトニ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ジカンガ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ススム</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ゴトノ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヘンコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チャットは30レスを各ルーム毎に表示</t>
+    <rPh sb="10" eb="11">
+      <t>カクルーｍ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ゴト</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30レス移行スクロールを行うと現在表示しているレス含め最大100レスを表示処理を行う。</t>
+    <rPh sb="4" eb="6">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>オコナウト</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>フクメ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>サイダイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ショリヲ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>オコナウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>API</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>更新タイミングは20秒毎に行う</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>オコナウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>課題</t>
+    <rPh sb="0" eb="2">
+      <t>カダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>同時に同じユーザーから複数アクセスがある場合のサーバサイドの対処</t>
+    <rPh sb="0" eb="2">
+      <t>ドウジ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>オナジ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>タイショ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サーバサイドメモ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バリデーション</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DevelopmentsServerURL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>www13054ue.sakura.ne.jp/chat/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フォルダ構成の調査</t>
+    <rPh sb="4" eb="6">
+      <t>コウセイノ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>チョウサ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MVCモデルを意識</t>
+    <rPh sb="7" eb="9">
+      <t>イシキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>管理画面の実装方法について</t>
+    <rPh sb="0" eb="4">
+      <t>カンリガメンノ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ジッソウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ホウホウニツイテ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>apiのテンプレート</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mongodbのテンプレート</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>暗号化実装のための想定</t>
+    <rPh sb="0" eb="3">
+      <t>アンゴウカ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジッソウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ソウテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>禁止用語関連の実装</t>
+    <rPh sb="0" eb="4">
+      <t>キンシヨウゴ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カンレン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ジッソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ルーム選択機能</t>
+    <rPh sb="3" eb="7">
+      <t>センタクキノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ネイティブ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サーバ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログイン時</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Guild,room,private</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>request（chat login）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>data 30 news(Guild,room,private)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>response</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mongoDB依存のID</t>
+    <rPh sb="7" eb="9">
+      <t>イゾンノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RoomID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ギルド、ルーム等のID</t>
+    <rPh sb="7" eb="8">
+      <t>トウノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int番号でルームID関わらずカウントする</t>
+    <rPh sb="3" eb="5">
+      <t>バンゴウデ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>カカワラズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CommentNo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>文字数制限はサーバー及びアプリケーションでValidationを行う</t>
+    <rPh sb="0" eb="3">
+      <t>モジスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セイゲンハ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>オヨビ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>オコナウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>コメント</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿した時の時刻を強いようする</t>
+    <rPh sb="0" eb="2">
+      <t>トウコウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジコクヲ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>シイヨウスル</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ISODate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ID：ISODate("2015-10-10T12:24:19Z")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザー名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UserID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿者のUserIDを記録</t>
+    <rPh sb="0" eb="3">
+      <t>トウコウシャノ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>キロク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DB設計</t>
+    <rPh sb="2" eb="4">
+      <t>セッケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mongoDBを使用して</t>
+    <rPh sb="8" eb="10">
+      <t>シヨウシテ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザー管理</t>
+    <rPh sb="4" eb="6">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IconID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チャット用のアイコンのID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ログイン時の処理</t>
+    <rPh sb="6" eb="8">
+      <t>ショリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>更新時の処理</t>
+    <rPh sb="0" eb="3">
+      <t>コウシンジ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ショリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>投稿時の処理</t>
+    <rPh sb="0" eb="3">
+      <t>トウコウジ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ショリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザー詳細の展開</t>
+    <rPh sb="4" eb="6">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>テンカイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>他の人のプライベートチャットへ</t>
+    <rPh sb="0" eb="1">
+      <t>ホカノヒトノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/chat/update</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/chat/user?userid=(intでUserID)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/chat/update_p?userid=(intでUserID)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/chat/login?userid=(intでUserID)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>/api/chat/update?userid=(intでUserID)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>受信時のパラメータ</t>
+    <rPh sb="0" eb="2">
+      <t>ジュシン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>送信時のパラメータ</t>
+    <rPh sb="0" eb="3">
+      <t>ソウシンジノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>privateRoomにアクセス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaaada</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>//php install</t>
+  </si>
+  <si>
+    <t>yum install epel-release</t>
+  </si>
+  <si>
+    <t>rpm -Uvh http://rpms.famillecollet.com/enterprise/remi-release-7.rpm</t>
+  </si>
+  <si>
+    <t>yum install --enablerepo=remi,remi-php70 php php-devel php-mbstring php-pdo php-gd</t>
+  </si>
+  <si>
+    <t>//php setting</t>
+  </si>
+  <si>
+    <t>vi /etc/php.ini</t>
+  </si>
+  <si>
+    <t>//mongodb install</t>
+  </si>
+  <si>
+    <t>vi /etc/yum.repos.d/mongodb-org-3.0.repo</t>
+  </si>
+  <si>
+    <t>&gt;[mongodb-org-3.0]</t>
+  </si>
+  <si>
+    <t>&gt;name=MongoDB Repository</t>
+  </si>
+  <si>
+    <t>&gt;baseurl=http://repo.mongodb.org/yum/redhat/$releasever/mongodb-org/3.0/x86_64/</t>
+  </si>
+  <si>
+    <t>&gt;gpgcheck=0</t>
+  </si>
+  <si>
+    <t>&gt;enabled=1</t>
+  </si>
+  <si>
+    <t>yum install mongodb-org</t>
+  </si>
+  <si>
+    <t>systemctl start mongod</t>
+  </si>
+  <si>
+    <t>systemctl stop mongod</t>
+  </si>
+  <si>
+    <t>chkconfig mongod on</t>
+  </si>
+  <si>
+    <t>//mariaDB install</t>
+  </si>
+  <si>
+    <t>vi /etc/yum.repos.d/MariaDB.repo</t>
+  </si>
+  <si>
+    <t>&gt;[mariadb]</t>
+  </si>
+  <si>
+    <t>&gt;name = MariaDB</t>
+  </si>
+  <si>
+    <t>&gt;baseurl = http://yum.mariadb.org/10.1/centos7-amd64</t>
+  </si>
+  <si>
+    <t>&gt;gpgkey=https://yum.mariadb.org/RPM-GPG-KEY-MariaDB</t>
+  </si>
+  <si>
+    <t>&gt;gpgcheck=1</t>
+  </si>
+  <si>
+    <t>yum install MariaDB-server MariaDB-client</t>
+  </si>
+  <si>
+    <t>systemctl start mariadb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//CentOS7 portfowarding </t>
+  </si>
+  <si>
+    <t>firewall-cmd --zone=external --add-port=3306/tcp</t>
+  </si>
+  <si>
+    <t>firewall-cmd --zone=external --add-port=3306/tcp --permanent</t>
+  </si>
+  <si>
+    <t>firewall-cmd --zone=external --add-port=27017/tcp</t>
+  </si>
+  <si>
+    <t>firewall-cmd --zone=external --add-port=27017/tcp --permanent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,6 +708,15 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
       <charset val="128"/>
@@ -144,8 +743,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -158,6 +758,361 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1130300" y="762000"/>
+          <a:ext cx="2273300" cy="4127500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5664200" y="762000"/>
+          <a:ext cx="2273300" cy="4127500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10160000" y="774700"/>
+          <a:ext cx="2273300" cy="4127500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="直線矢印コネクタ 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3403600" y="1270000"/>
+          <a:ext cx="2260600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="直線矢印コネクタ 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="1485900"/>
+          <a:ext cx="2260600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="直線矢印コネクタ 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7962900" y="2286000"/>
+          <a:ext cx="2209800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直線矢印コネクタ 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3429000" y="2552700"/>
+          <a:ext cx="2209800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,30 +1378,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -454,22 +1409,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -480,17 +1435,137 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>27017</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
+      </c>
+      <c r="E12">
+        <v>3306</v>
+      </c>
+      <c r="P12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -500,6 +1575,177 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -512,19 +1758,338 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>